<commit_message>
Updating recall sheets by sorting alphabetically and adding scoring fields by living/non-living
</commit_message>
<xml_diff>
--- a/various/recallSheet1.xlsx
+++ b/various/recallSheet1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>List</t>
   </si>
@@ -335,16 +335,34 @@
     <t xml:space="preserve">APRON </t>
   </si>
   <si>
-    <t>Intrusions:</t>
-  </si>
-  <si>
-    <t>Number of words recalled</t>
-  </si>
-  <si>
-    <t>Number of intrusions</t>
-  </si>
-  <si>
     <t>Free recall sheet for noveltyVR</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Living words</t>
+  </si>
+  <si>
+    <t>Non-living words</t>
+  </si>
+  <si>
+    <t>Living Recalled:</t>
+  </si>
+  <si>
+    <t>Non-living Recalled:</t>
+  </si>
+  <si>
+    <t>Total number recalled:</t>
+  </si>
+  <si>
+    <t>Total number intrusions:</t>
+  </si>
+  <si>
+    <t>Living Intrusions:</t>
+  </si>
+  <si>
+    <t>Non-living Intrusions:</t>
   </si>
 </sst>
 </file>
@@ -415,37 +433,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -600,21 +587,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -657,6 +629,54 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -667,6 +687,32 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -677,34 +723,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -733,6 +755,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -741,8 +765,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,527 +1060,555 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
+      <c r="H29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="24"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25"/>
+    </row>
+    <row r="52" spans="13:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M52" s="11"/>
     </row>
   </sheetData>
+  <sortState ref="M2:M52">
+    <sortCondition ref="M2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>